<commit_message>
Added glossary for year 1 and changed the code a bit
</commit_message>
<xml_diff>
--- a/book/glossary/Glossary_CT.xlsx
+++ b/book/glossary/Glossary_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\werel\Documents\P-RE-CONNECT\ECT_Book\book\glossary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{11AFB3DC-FA62-44CB-9F26-18886515A253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72D75E5-43F7-4BC7-AF43-8B3C696D7C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Greek Symbols" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="343">
   <si>
     <t>Symbol</t>
   </si>
@@ -386,15 +386,6 @@
     <t>$\dot{\theta}$</t>
   </si>
   <si>
-    <t>Angle (argument of z)</t>
-  </si>
-  <si>
-    <t>Modulus or magnitude</t>
-  </si>
-  <si>
-    <t>Discriminant</t>
-  </si>
-  <si>
     <t>Damping coefficient</t>
   </si>
   <si>
@@ -555,16 +546,533 @@
   </si>
   <si>
     <t>Approximately equal to</t>
+  </si>
+  <si>
+    <t>Riemann sum</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>$\bar{x}$</t>
+  </si>
+  <si>
+    <t>$\bar{y}$</t>
+  </si>
+  <si>
+    <t>x-coordinate of center of mass</t>
+  </si>
+  <si>
+    <t>y-coordinate of center of mass</t>
+  </si>
+  <si>
+    <t>Discriminant, domain</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Modulus or magnitude, radial distance (polar coordinate)</t>
+  </si>
+  <si>
+    <t>(polar) angle (argument of z)</t>
+  </si>
+  <si>
+    <t>Azimuthal angle</t>
+  </si>
+  <si>
+    <t>$I_{x}$</t>
+  </si>
+  <si>
+    <t>Moment of inertia around the x-axis</t>
+  </si>
+  <si>
+    <t>Moment of inertia around the y-axis</t>
+  </si>
+  <si>
+    <t>Moment of inertia around the z-axis</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>$\vec{b}$</t>
+  </si>
+  <si>
+    <t>Vector b</t>
+  </si>
+  <si>
+    <t>$\vec{x}$</t>
+  </si>
+  <si>
+    <t>Vector x</t>
+  </si>
+  <si>
+    <t>Number of rows in a matrix</t>
+  </si>
+  <si>
+    <t>Number of columns in a matrix</t>
+  </si>
+  <si>
+    <t>Transformation</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>$A^T$</t>
+  </si>
+  <si>
+    <t>Matrix transpose</t>
+  </si>
+  <si>
+    <t>$Col A$</t>
+  </si>
+  <si>
+    <t>$nul A$</t>
+  </si>
+  <si>
+    <t>Null space of a matrix</t>
+  </si>
+  <si>
+    <t>Column space of a matrix</t>
+  </si>
+  <si>
+    <t>$\perp$</t>
+  </si>
+  <si>
+    <t>Perpendicular/orthogonal</t>
+  </si>
+  <si>
+    <t>Stress</t>
+  </si>
+  <si>
+    <t>Normal force</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Young's modulus</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Length difference</t>
+  </si>
+  <si>
+    <t>Tensile stiffness</t>
+  </si>
+  <si>
+    <t>Bending stiffness</t>
+  </si>
+  <si>
+    <t>Displacement</t>
+  </si>
+  <si>
+    <t>Distributed force</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>$S_z$</t>
+  </si>
+  <si>
+    <t>First moment of inertia (static moment)</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Moment of inertia around z-axis</t>
+  </si>
+  <si>
+    <t>Moment/torsion</t>
+  </si>
+  <si>
+    <t>Shear force</t>
+  </si>
+  <si>
+    <t>Rotation</t>
+  </si>
+  <si>
+    <t>Curvature</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Eccentricity</t>
+  </si>
+  <si>
+    <t>Horizontal shear flow</t>
+  </si>
+  <si>
+    <t>Shear stress</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Radius (of curvature)</t>
+  </si>
+  <si>
+    <t>Torsional moment</t>
+  </si>
+  <si>
+    <t>Polar moment of inertia</t>
+  </si>
+  <si>
+    <t>Phase strength</t>
+  </si>
+  <si>
+    <t>$f_v$</t>
+  </si>
+  <si>
+    <t>Volume fraction</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Fineness modulus</t>
+  </si>
+  <si>
+    <t>Moisture content</t>
+  </si>
+  <si>
+    <t>Number of atoms</t>
+  </si>
+  <si>
+    <t>Atomic mass</t>
+  </si>
+  <si>
+    <t>$N_A$</t>
+  </si>
+  <si>
+    <t>Avogadro's number</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>Poisson's ratio</t>
+  </si>
+  <si>
+    <t>Shear modulus</t>
+  </si>
+  <si>
+    <t>Shear angle</t>
+  </si>
+  <si>
+    <t>Crack length</t>
+  </si>
+  <si>
+    <t>Total surface energy</t>
+  </si>
+  <si>
+    <t>$\sigma'$</t>
+  </si>
+  <si>
+    <t>Stress at crack tip</t>
+  </si>
+  <si>
+    <t>$\sigma_o$</t>
+  </si>
+  <si>
+    <t>Stress applied on the surface</t>
+  </si>
+  <si>
+    <t>Identify matrix</t>
+  </si>
+  <si>
+    <t>Eigenvalue</t>
+  </si>
+  <si>
+    <t>$\Epsilon_{\lambda}$</t>
+  </si>
+  <si>
+    <t>Eigenspace</t>
+  </si>
+  <si>
+    <t>$\vec{v}$</t>
+  </si>
+  <si>
+    <t>Eigenvector</t>
+  </si>
+  <si>
+    <t>Real part</t>
+  </si>
+  <si>
+    <t>Imaginary part</t>
+  </si>
+  <si>
+    <t>Quadratic form</t>
+  </si>
+  <si>
+    <t>Moment</t>
+  </si>
+  <si>
+    <t>Section modulus</t>
+  </si>
+  <si>
+    <t>Mass moment of inertia</t>
+  </si>
+  <si>
+    <t>$S_a$</t>
+  </si>
+  <si>
+    <t>Static moment</t>
+  </si>
+  <si>
+    <t>$l_k$</t>
+  </si>
+  <si>
+    <t>Buckling Length</t>
+  </si>
+  <si>
+    <t>Ultimate limit state</t>
+  </si>
+  <si>
+    <t>Serviceability limit state</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Stress, standard deviation</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
+  <si>
+    <t>$x$</t>
+  </si>
+  <si>
+    <t>Compression zone</t>
+  </si>
+  <si>
+    <t>$\sigma_v$</t>
+  </si>
+  <si>
+    <t>Total vertical stress</t>
+  </si>
+  <si>
+    <t>Bulk unit weight</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Vertical effective stress</t>
+  </si>
+  <si>
+    <t>Pore water pressure</t>
+  </si>
+  <si>
+    <t>Cohesion</t>
+  </si>
+  <si>
+    <t>Angle of internal friction</t>
+  </si>
+  <si>
+    <t>$\tau_f$</t>
+  </si>
+  <si>
+    <t>Failure shear stress</t>
+  </si>
+  <si>
+    <t>Effective height, diameter</t>
+  </si>
+  <si>
+    <t>Friction ratio</t>
+  </si>
+  <si>
+    <t>$f_cs$</t>
+  </si>
+  <si>
+    <t>Cone resistance</t>
+  </si>
+  <si>
+    <t>Sleeve/side friction</t>
+  </si>
+  <si>
+    <t>$B_a$</t>
+  </si>
+  <si>
+    <t>Pore pressure ratio</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>$q_n$</t>
+  </si>
+  <si>
+    <t>Net cone resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$D_r$ </t>
+  </si>
+  <si>
+    <t>Relative density</t>
+  </si>
+  <si>
+    <t>$S_u$</t>
+  </si>
+  <si>
+    <t>Undrained strenght</t>
+  </si>
+  <si>
+    <t>$Q_t$</t>
+  </si>
+  <si>
+    <t>Total capacity</t>
+  </si>
+  <si>
+    <t>$q_b$</t>
+  </si>
+  <si>
+    <t>Base resistance</t>
+  </si>
+  <si>
+    <t>$Q_s$</t>
+  </si>
+  <si>
+    <t>Shaft resistance</t>
+  </si>
+  <si>
+    <t>$Q_b$</t>
+  </si>
+  <si>
+    <t>Thermal expansion coefficient, emperical base factor</t>
+  </si>
+  <si>
+    <t>Factor for enlarged pile bases</t>
+  </si>
+  <si>
+    <t>Cross-sectional shape reduction factor</t>
+  </si>
+  <si>
+    <t>$k_0$</t>
+  </si>
+  <si>
+    <t>Interface friction angle between the soil and pile</t>
+  </si>
+  <si>
+    <t>Coefficient for earth pressure at rest</t>
+  </si>
+  <si>
+    <t>Operational earth pressure coefficient</t>
+  </si>
+  <si>
+    <t>$N_q$</t>
+  </si>
+  <si>
+    <t>Bearing capacity factor</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Usefulness of alternative</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>$B$</t>
+  </si>
+  <si>
+    <t>Benefits</t>
+  </si>
+  <si>
+    <t>Arc radius</t>
+  </si>
+  <si>
+    <t>Design velocity</t>
+  </si>
+  <si>
+    <t>Parameter for clotoïde</t>
+  </si>
+  <si>
+    <t>Centripetal force</t>
+  </si>
+  <si>
+    <t>Angular rotation</t>
+  </si>
+  <si>
+    <t>Reference viewing distance</t>
+  </si>
+  <si>
+    <t>Discount rate, gradient</t>
+  </si>
+  <si>
+    <t>Acceleration</t>
+  </si>
+  <si>
+    <t>Mean following distance</t>
+  </si>
+  <si>
+    <t>Height, mean following time</t>
+  </si>
+  <si>
+    <t>Mean velocity</t>
+  </si>
+  <si>
+    <t>Intensity</t>
+  </si>
+  <si>
+    <t>Shock wave speed</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -590,8 +1098,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,24 +1381,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2617A03-EA22-4211-801A-355FACE4DDAC}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="42.28515625" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -964,16 +1473,28 @@
       <c r="A3" t="s">
         <v>21</v>
       </c>
+      <c r="J3" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
+      <c r="J4" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>95</v>
       </c>
+      <c r="I5" t="s">
+        <v>250</v>
+      </c>
+      <c r="J5" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -984,116 +1505,237 @@
       <c r="A7" t="s">
         <v>97</v>
       </c>
+      <c r="J7" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>99</v>
       </c>
+      <c r="H9" t="s">
+        <v>211</v>
+      </c>
+      <c r="I9" t="s">
+        <v>211</v>
+      </c>
+      <c r="J9" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>100</v>
       </c>
+      <c r="H10" t="s">
+        <v>210</v>
+      </c>
+      <c r="I10" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>259</v>
+      </c>
+      <c r="I11" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
+        <v>184</v>
+      </c>
+      <c r="H14" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="H17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="I18" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="J19" t="s">
+        <v>275</v>
+      </c>
+      <c r="K19" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="I20" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>176</v>
+      </c>
+      <c r="I22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="H23" t="s">
+        <v>207</v>
+      </c>
+      <c r="I23" t="s">
+        <v>236</v>
+      </c>
+      <c r="J23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>253</v>
+      </c>
+      <c r="I24" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I25" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>281</v>
+      </c>
+      <c r="J26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="J27" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="H28" t="s">
+        <v>231</v>
+      </c>
+      <c r="I28" t="s">
+        <v>231</v>
+      </c>
+      <c r="J28" t="s">
+        <v>231</v>
+      </c>
+      <c r="K28" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>289</v>
+      </c>
+      <c r="J29" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B30" t="s">
+        <v>185</v>
+      </c>
+      <c r="G30" t="s">
+        <v>198</v>
+      </c>
+      <c r="H30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="J31" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>116</v>
+      </c>
+      <c r="K33" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -1104,10 +1746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B66207E-F3A7-4A76-96AD-A5712E9C1247}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,208 +1762,216 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1332,25 +1982,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="42.28515625" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1425,366 +2075,891 @@
       <c r="A3" t="s">
         <v>93</v>
       </c>
+      <c r="G3" t="s">
+        <v>263</v>
+      </c>
+      <c r="H3" t="s">
+        <v>218</v>
+      </c>
+      <c r="I3" t="s">
+        <v>251</v>
+      </c>
+      <c r="K3" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
+      <c r="G4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H4" t="s">
+        <v>209</v>
+      </c>
+      <c r="I4" t="s">
+        <v>244</v>
+      </c>
+      <c r="J4" t="s">
+        <v>209</v>
+      </c>
+      <c r="K4" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>199</v>
+      </c>
+      <c r="G5" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>122</v>
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H6" t="s">
+        <v>221</v>
+      </c>
+      <c r="J6" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>191</v>
+      </c>
+      <c r="G7" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>326</v>
+      </c>
+      <c r="K8" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>121</v>
+        <v>296</v>
+      </c>
+      <c r="J9" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" t="s">
+        <v>287</v>
+      </c>
+      <c r="K10" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>201</v>
+      </c>
+      <c r="G12" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>240</v>
+      </c>
+      <c r="J13" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>181</v>
+      </c>
+      <c r="J14" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>301</v>
+      </c>
+      <c r="J15" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" t="s">
+        <v>210</v>
+      </c>
+      <c r="I17" t="s">
+        <v>210</v>
+      </c>
+      <c r="J17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" t="s">
+        <v>215</v>
+      </c>
+      <c r="J19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>293</v>
+      </c>
+      <c r="J21" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>237</v>
+      </c>
+      <c r="I22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="H24" t="s">
+        <v>228</v>
+      </c>
+      <c r="J24" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="I26" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="I28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="H29" t="s">
+        <v>222</v>
+      </c>
+      <c r="J29" t="s">
+        <v>222</v>
+      </c>
+      <c r="K29" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="J31" t="s">
+        <v>284</v>
+      </c>
+      <c r="K31" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>43</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B33" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="G33" t="s">
+        <v>92</v>
+      </c>
+      <c r="K33" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="G34" t="s">
+        <v>257</v>
+      </c>
+      <c r="J34" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="H35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B37" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="H38" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B39" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="H40" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="J42" t="s">
+        <v>318</v>
+      </c>
+      <c r="K42" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>315</v>
+      </c>
+      <c r="J43" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="K44" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="H45" t="s">
+        <v>212</v>
+      </c>
+      <c r="I45" t="s">
+        <v>212</v>
+      </c>
+      <c r="J45" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>271</v>
+      </c>
+      <c r="J46" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="H47" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="K48" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B49" t="s">
+        <v>175</v>
+      </c>
+      <c r="G49" t="s">
+        <v>195</v>
+      </c>
+      <c r="I49" t="s">
+        <v>175</v>
+      </c>
+      <c r="K49" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="H50" t="s">
+        <v>224</v>
+      </c>
+      <c r="J50" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="H51" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="G52" t="s">
+        <v>196</v>
+      </c>
+      <c r="I52" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>202</v>
+      </c>
+      <c r="G53" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="H55" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>245</v>
+      </c>
+      <c r="I56" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>319</v>
+      </c>
+      <c r="J57" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="K59" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="J60" t="s">
+        <v>298</v>
+      </c>
+      <c r="K60" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="H61" t="s">
+        <v>217</v>
+      </c>
+      <c r="K61" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>307</v>
+      </c>
+      <c r="J62" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="J63" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>299</v>
+      </c>
+      <c r="J64" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="G65" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>311</v>
+      </c>
+      <c r="J66" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>309</v>
+      </c>
+      <c r="J67" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>305</v>
+      </c>
+      <c r="J68" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>68</v>
       </c>
-      <c r="B50" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B69" t="s">
+        <v>183</v>
+      </c>
+      <c r="I69" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="H70" t="s">
+        <v>233</v>
+      </c>
+      <c r="J70" t="s">
+        <v>278</v>
+      </c>
+      <c r="K70" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="J72" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="J73" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="H74" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B75" t="s">
+        <v>173</v>
+      </c>
+      <c r="I75" t="s">
+        <v>252</v>
+      </c>
+      <c r="J75" t="s">
+        <v>277</v>
+      </c>
+      <c r="K75" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>269</v>
+      </c>
+      <c r="J76" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>303</v>
+      </c>
+      <c r="J77" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>219</v>
+      </c>
+      <c r="H78" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="J79" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="H80" t="s">
+        <v>232</v>
+      </c>
+      <c r="K80" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="G81" t="s">
+        <v>197</v>
+      </c>
+      <c r="H81" t="s">
+        <v>224</v>
+      </c>
+      <c r="I81" t="s">
+        <v>239</v>
+      </c>
+      <c r="J81" t="s">
+        <v>239</v>
+      </c>
+      <c r="K81" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="H82" t="s">
+        <v>216</v>
+      </c>
+      <c r="J82" t="s">
+        <v>286</v>
+      </c>
+      <c r="K82" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="J84" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="K85" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>261</v>
+      </c>
+      <c r="G86" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="B87" t="s">
+        <v>182</v>
+      </c>
+      <c r="H87" t="s">
+        <v>225</v>
+      </c>
+      <c r="I87" t="s">
+        <v>182</v>
+      </c>
+      <c r="J87" t="s">
+        <v>225</v>
+      </c>
+      <c r="K87" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="H88" t="s">
+        <v>216</v>
+      </c>
+      <c r="I88" t="s">
+        <v>242</v>
+      </c>
+      <c r="J88" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="J89" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>279</v>
+      </c>
+      <c r="J94" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>177</v>
+      </c>
+      <c r="B95" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>193</v>
+      </c>
+      <c r="G96" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>178</v>
+      </c>
+      <c r="B98" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="H99" t="s">
+        <v>218</v>
+      </c>
+      <c r="K99" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added code for interactive glossary in a .py file
</commit_message>
<xml_diff>
--- a/book/glossary/Glossary_CT.xlsx
+++ b/book/glossary/Glossary_CT.xlsx
@@ -8,26 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\werel\Documents\P-RE-CONNECT\ECT_Book\book\glossary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72D75E5-43F7-4BC7-AF43-8B3C696D7C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CBEC5F-4FB4-4785-9002-B6D9F4E45CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Greek Symbols" sheetId="2" r:id="rId1"/>
     <sheet name="Math Operators" sheetId="3" r:id="rId2"/>
     <sheet name="Latin Symbols" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="369">
   <si>
     <t>Symbol</t>
   </si>
@@ -1056,6 +1067,84 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Epsilon</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>kappa</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>nu</t>
+  </si>
+  <si>
+    <t>xi</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>omega</t>
+  </si>
+  <si>
+    <t>gamma dot</t>
+  </si>
+  <si>
+    <t>epsilon</t>
+  </si>
+  <si>
+    <t>Epsilon_lambda</t>
+  </si>
+  <si>
+    <t>theta dot</t>
+  </si>
+  <si>
+    <t>theta double dot</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1381,148 +1470,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2617A03-EA22-4211-801A-355FACE4DDAC}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="42.28515625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" customWidth="1"/>
+    <col min="11" max="11" width="42.28515625" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
+      <c r="B3" t="s">
+        <v>345</v>
+      </c>
+      <c r="K3" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
-      <c r="J4" t="s">
+      <c r="B4" t="s">
+        <v>346</v>
+      </c>
+      <c r="K4" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>95</v>
       </c>
-      <c r="I5" t="s">
+      <c r="B5" t="s">
+        <v>347</v>
+      </c>
+      <c r="J5" t="s">
         <v>250</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>97</v>
       </c>
-      <c r="J7" t="s">
+      <c r="B7" t="s">
+        <v>348</v>
+      </c>
+      <c r="K7" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>98</v>
       </c>
       <c r="B8" t="s">
+        <v>343</v>
+      </c>
+      <c r="C8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>99</v>
       </c>
-      <c r="H9" t="s">
-        <v>211</v>
+      <c r="B9" t="s">
+        <v>364</v>
       </c>
       <c r="I9" t="s">
         <v>211</v>
@@ -1530,160 +1641,217 @@
       <c r="J9" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>100</v>
       </c>
-      <c r="H10" t="s">
-        <v>210</v>
+      <c r="B10" t="s">
+        <v>344</v>
       </c>
       <c r="I10" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>259</v>
       </c>
-      <c r="I11" t="s">
+      <c r="B11" t="s">
+        <v>365</v>
+      </c>
+      <c r="J11" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>103</v>
       </c>
       <c r="B14" t="s">
+        <v>351</v>
+      </c>
+      <c r="C14" t="s">
         <v>184</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>104</v>
       </c>
-      <c r="H17" t="s">
+      <c r="B17" t="s">
+        <v>352</v>
+      </c>
+      <c r="I17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>105</v>
       </c>
-      <c r="I18" t="s">
+      <c r="B18" t="s">
+        <v>353</v>
+      </c>
+      <c r="J18" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>106</v>
       </c>
-      <c r="J19" t="s">
+      <c r="B19" t="s">
+        <v>354</v>
+      </c>
+      <c r="K19" t="s">
         <v>275</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>107</v>
       </c>
-      <c r="I20" t="s">
+      <c r="B20" t="s">
+        <v>355</v>
+      </c>
+      <c r="J20" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>109</v>
       </c>
       <c r="B22" t="s">
+        <v>357</v>
+      </c>
+      <c r="C22" t="s">
         <v>176</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>110</v>
       </c>
-      <c r="H23" t="s">
+      <c r="B23" t="s">
+        <v>358</v>
+      </c>
+      <c r="I23" t="s">
         <v>207</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>236</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>253</v>
       </c>
-      <c r="I24" t="s">
+      <c r="B24" t="s">
+        <v>358</v>
+      </c>
+      <c r="J24" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="I25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="J25" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>281</v>
       </c>
-      <c r="J26" t="s">
+      <c r="B26" t="s">
+        <v>358</v>
+      </c>
+      <c r="K26" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>111</v>
       </c>
-      <c r="J27" t="s">
+      <c r="B27" t="s">
+        <v>358</v>
+      </c>
+      <c r="K27" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>112</v>
       </c>
-      <c r="H28" t="s">
-        <v>231</v>
+      <c r="B28" t="s">
+        <v>359</v>
       </c>
       <c r="I28" t="s">
         <v>231</v>
@@ -1692,49 +1860,67 @@
         <v>231</v>
       </c>
       <c r="K28" t="s">
+        <v>231</v>
+      </c>
+      <c r="L28" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>289</v>
       </c>
-      <c r="J29" t="s">
+      <c r="B29" t="s">
+        <v>359</v>
+      </c>
+      <c r="K29" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>114</v>
       </c>
       <c r="B30" t="s">
+        <v>360</v>
+      </c>
+      <c r="C30" t="s">
         <v>185</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>198</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
-      <c r="J31" t="s">
+      <c r="B31" t="s">
+        <v>360</v>
+      </c>
+      <c r="K31" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>116</v>
       </c>
-      <c r="K33" t="s">
+      <c r="B33" t="s">
+        <v>362</v>
+      </c>
+      <c r="L33" t="s">
         <v>340</v>
       </c>
     </row>
@@ -1748,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B66207E-F3A7-4A76-96AD-A5712E9C1247}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,6 +1980,9 @@
       <c r="A4" t="s">
         <v>127</v>
       </c>
+      <c r="B4" t="s">
+        <v>368</v>
+      </c>
       <c r="C4" t="s">
         <v>128</v>
       </c>
@@ -1802,6 +1991,9 @@
       <c r="A5" t="s">
         <v>131</v>
       </c>
+      <c r="B5" t="s">
+        <v>368</v>
+      </c>
       <c r="C5" t="s">
         <v>132</v>
       </c>
@@ -1810,6 +2002,9 @@
       <c r="A6" t="s">
         <v>133</v>
       </c>
+      <c r="B6" t="s">
+        <v>368</v>
+      </c>
       <c r="C6" t="s">
         <v>134</v>
       </c>
@@ -1818,6 +2013,9 @@
       <c r="A7" t="s">
         <v>135</v>
       </c>
+      <c r="B7" t="s">
+        <v>368</v>
+      </c>
       <c r="C7" t="s">
         <v>136</v>
       </c>
@@ -1826,6 +2024,9 @@
       <c r="A8" t="s">
         <v>137</v>
       </c>
+      <c r="B8" t="s">
+        <v>368</v>
+      </c>
       <c r="C8" t="s">
         <v>138</v>
       </c>
@@ -1834,6 +2035,9 @@
       <c r="A9" t="s">
         <v>139</v>
       </c>
+      <c r="B9" t="s">
+        <v>368</v>
+      </c>
       <c r="C9" t="s">
         <v>140</v>
       </c>
@@ -1842,6 +2046,9 @@
       <c r="A10" t="s">
         <v>153</v>
       </c>
+      <c r="B10" t="s">
+        <v>368</v>
+      </c>
       <c r="C10" t="s">
         <v>141</v>
       </c>
@@ -1850,6 +2057,9 @@
       <c r="A11" t="s">
         <v>154</v>
       </c>
+      <c r="B11" t="s">
+        <v>368</v>
+      </c>
       <c r="C11" t="s">
         <v>142</v>
       </c>
@@ -1858,6 +2068,9 @@
       <c r="A12" t="s">
         <v>155</v>
       </c>
+      <c r="B12" t="s">
+        <v>368</v>
+      </c>
       <c r="C12" t="s">
         <v>143</v>
       </c>
@@ -1866,6 +2079,9 @@
       <c r="A13" t="s">
         <v>156</v>
       </c>
+      <c r="B13" t="s">
+        <v>368</v>
+      </c>
       <c r="C13" t="s">
         <v>144</v>
       </c>
@@ -1874,6 +2090,9 @@
       <c r="A14" t="s">
         <v>157</v>
       </c>
+      <c r="B14" t="s">
+        <v>368</v>
+      </c>
       <c r="C14" t="s">
         <v>158</v>
       </c>
@@ -1882,6 +2101,9 @@
       <c r="A15" t="s">
         <v>159</v>
       </c>
+      <c r="B15" t="s">
+        <v>368</v>
+      </c>
       <c r="C15" t="s">
         <v>145</v>
       </c>
@@ -1890,6 +2112,9 @@
       <c r="A16" t="s">
         <v>160</v>
       </c>
+      <c r="B16" t="s">
+        <v>368</v>
+      </c>
       <c r="C16" t="s">
         <v>161</v>
       </c>
@@ -1898,6 +2123,9 @@
       <c r="A17" t="s">
         <v>162</v>
       </c>
+      <c r="B17" t="s">
+        <v>368</v>
+      </c>
       <c r="C17" t="s">
         <v>146</v>
       </c>
@@ -1906,6 +2134,9 @@
       <c r="A18" t="s">
         <v>163</v>
       </c>
+      <c r="B18" t="s">
+        <v>368</v>
+      </c>
       <c r="C18" t="s">
         <v>147</v>
       </c>
@@ -1914,6 +2145,9 @@
       <c r="A19" t="s">
         <v>164</v>
       </c>
+      <c r="B19" t="s">
+        <v>368</v>
+      </c>
       <c r="C19" t="s">
         <v>148</v>
       </c>
@@ -1922,6 +2156,9 @@
       <c r="A20" t="s">
         <v>165</v>
       </c>
+      <c r="B20" t="s">
+        <v>368</v>
+      </c>
       <c r="C20" t="s">
         <v>149</v>
       </c>
@@ -1930,6 +2167,9 @@
       <c r="A21" t="s">
         <v>166</v>
       </c>
+      <c r="B21" t="s">
+        <v>368</v>
+      </c>
       <c r="C21" t="s">
         <v>150</v>
       </c>
@@ -1938,6 +2178,9 @@
       <c r="A22" t="s">
         <v>167</v>
       </c>
+      <c r="B22" t="s">
+        <v>368</v>
+      </c>
       <c r="C22" t="s">
         <v>168</v>
       </c>
@@ -1946,6 +2189,9 @@
       <c r="A23" t="s">
         <v>169</v>
       </c>
+      <c r="B23" t="s">
+        <v>368</v>
+      </c>
       <c r="C23" t="s">
         <v>151</v>
       </c>
@@ -1954,6 +2200,9 @@
       <c r="A24" t="s">
         <v>170</v>
       </c>
+      <c r="B24" t="s">
+        <v>368</v>
+      </c>
       <c r="C24" t="s">
         <v>152</v>
       </c>
@@ -1962,6 +2211,9 @@
       <c r="A25" t="s">
         <v>171</v>
       </c>
+      <c r="B25" t="s">
+        <v>368</v>
+      </c>
       <c r="C25" t="s">
         <v>172</v>
       </c>
@@ -1969,6 +2221,9 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>205</v>
+      </c>
+      <c r="B26" t="s">
+        <v>368</v>
       </c>
       <c r="C26" t="s">
         <v>206</v>
@@ -1984,7 +2239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>

</xml_diff>

<commit_message>
Added Q2 Year 2 CT Bachelor and changed code for interactive table
</commit_message>
<xml_diff>
--- a/book/glossary/Glossary_CT.xlsx
+++ b/book/glossary/Glossary_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\werel\Documents\P-RE-CONNECT\ECT_Book\book\glossary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A08C3D-3A22-46EB-B063-47AABBE8301F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D9A108-DD40-4ABB-AF93-891359D5D866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Greek Symbols" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="552">
   <si>
     <t>Symbol</t>
   </si>
@@ -1445,6 +1445,255 @@
   </si>
   <si>
     <t>Rate, radius</t>
+  </si>
+  <si>
+    <t>$IQR$</t>
+  </si>
+  <si>
+    <t>Interquartile range</t>
+  </si>
+  <si>
+    <t>Number of datapoints</t>
+  </si>
+  <si>
+    <t>$\Omega$</t>
+  </si>
+  <si>
+    <t>Omega</t>
+  </si>
+  <si>
+    <t>Sample space</t>
+  </si>
+  <si>
+    <t>$\cup$</t>
+  </si>
+  <si>
+    <t>Union</t>
+  </si>
+  <si>
+    <t>$\cap$</t>
+  </si>
+  <si>
+    <t>Intersect</t>
+  </si>
+  <si>
+    <t>$\infty$</t>
+  </si>
+  <si>
+    <t>Infinity</t>
+  </si>
+  <si>
+    <t>Probability density function</t>
+  </si>
+  <si>
+    <t>Cumulative probability function</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>$\sigma^2$</t>
+  </si>
+  <si>
+    <t>sigma squared</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Normal distribution</t>
+  </si>
+  <si>
+    <t>Expectation</t>
+  </si>
+  <si>
+    <t>$Cov$</t>
+  </si>
+  <si>
+    <t>Covariance</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Random variable</t>
+  </si>
+  <si>
+    <t>Average of RV</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Estimator</t>
+  </si>
+  <si>
+    <t>$S_n$</t>
+  </si>
+  <si>
+    <t>Sample standard deviation</t>
+  </si>
+  <si>
+    <t>$S_p$</t>
+  </si>
+  <si>
+    <t>Node-sum-of-squares</t>
+  </si>
+  <si>
+    <t>Confidence level</t>
+  </si>
+  <si>
+    <t>Hypothesis</t>
+  </si>
+  <si>
+    <t>Likelihood function</t>
+  </si>
+  <si>
+    <t>Log-likelihood</t>
+  </si>
+  <si>
+    <t>Distributed load</t>
+  </si>
+  <si>
+    <t>$\delta \theta$</t>
+  </si>
+  <si>
+    <t>delta theta</t>
+  </si>
+  <si>
+    <t>Virtual rotation</t>
+  </si>
+  <si>
+    <t>Thermal expansion coefficient</t>
+  </si>
+  <si>
+    <t>Temperature, torsion</t>
+  </si>
+  <si>
+    <t>Spring stiffness</t>
+  </si>
+  <si>
+    <t>$F_k$</t>
+  </si>
+  <si>
+    <t>Buckling force</t>
+  </si>
+  <si>
+    <t>Buckling length</t>
+  </si>
+  <si>
+    <t>Ratio between $F_k$ and $F$</t>
+  </si>
+  <si>
+    <t>Mass inertia around z-axis</t>
+  </si>
+  <si>
+    <t>Mass inertia around y-axis</t>
+  </si>
+  <si>
+    <t>Normal stress</t>
+  </si>
+  <si>
+    <t>Reliability index</t>
+  </si>
+  <si>
+    <t>Performance function</t>
+  </si>
+  <si>
+    <t>Partial factor</t>
+  </si>
+  <si>
+    <t>$\Psi$</t>
+  </si>
+  <si>
+    <t>Psi</t>
+  </si>
+  <si>
+    <t>Combination factor</t>
+  </si>
+  <si>
+    <t>Variable loading</t>
+  </si>
+  <si>
+    <t>Accidental loading, area</t>
+  </si>
+  <si>
+    <t>Weld throat</t>
+  </si>
+  <si>
+    <t>Effects, young's modulus</t>
+  </si>
+  <si>
+    <t>Yield strength</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Permanent loading, shear modulus</t>
+  </si>
+  <si>
+    <t>$I_t$</t>
+  </si>
+  <si>
+    <t>Torsional moment of inertia</t>
+  </si>
+  <si>
+    <t>$I_w$</t>
+  </si>
+  <si>
+    <t>Warping constant</t>
+  </si>
+  <si>
+    <t>Standard deviation, normal stress</t>
+  </si>
+  <si>
+    <t>Sectio modulus</t>
+  </si>
+  <si>
+    <t>Radius of gyration</t>
+  </si>
+  <si>
+    <t>First moment of inertia</t>
+  </si>
+  <si>
+    <t>Slenderness</t>
+  </si>
+  <si>
+    <t>Reduction factor</t>
+  </si>
+  <si>
+    <t>Concrete cover</t>
+  </si>
+  <si>
+    <t>Density, reinforcement ratio</t>
+  </si>
+  <si>
+    <t>Reinforcement diameter</t>
+  </si>
+  <si>
+    <t>Diameter, effective height, design</t>
+  </si>
+  <si>
+    <t>Characteristic</t>
+  </si>
+  <si>
+    <t>Height of concrete compression zone</t>
+  </si>
+  <si>
+    <t>Shape factor, reduction factor</t>
+  </si>
+  <si>
+    <t>Internal lever arm</t>
+  </si>
+  <si>
+    <t>Shear strength</t>
+  </si>
+  <si>
+    <t>Crack width</t>
+  </si>
+  <si>
+    <t>Ratio between $F_k$ and $F$, relative normal force</t>
   </si>
 </sst>
 </file>
@@ -1773,12 +2022,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2617A03-EA22-4211-801A-355FACE4DDAC}">
-  <dimension ref="A1:X34"/>
+  <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
+      <selection pane="bottomLeft" activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,10 +2046,10 @@
     <col min="12" max="12" width="19.7109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="25.5703125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="28.7109375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="32" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="24" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="28.42578125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="31.28515625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="42.28515625" bestFit="1" customWidth="1"/>
@@ -1995,6 +2244,12 @@
       <c r="O4" t="s">
         <v>198</v>
       </c>
+      <c r="Q4" t="s">
+        <v>508</v>
+      </c>
+      <c r="R4" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2006,6 +2261,9 @@
       <c r="K5" t="s">
         <v>313</v>
       </c>
+      <c r="R5" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2026,6 +2284,12 @@
       <c r="N6" t="s">
         <v>250</v>
       </c>
+      <c r="P6" t="s">
+        <v>500</v>
+      </c>
+      <c r="R6" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2051,345 +2315,449 @@
       <c r="M8" t="s">
         <v>403</v>
       </c>
+      <c r="R8" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>505</v>
       </c>
       <c r="B9" t="s">
-        <v>343</v>
-      </c>
-      <c r="C9" t="s">
-        <v>120</v>
+        <v>506</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>364</v>
-      </c>
-      <c r="I10" t="s">
-        <v>211</v>
-      </c>
-      <c r="J10" t="s">
-        <v>211</v>
-      </c>
-      <c r="K10" t="s">
-        <v>211</v>
+        <v>343</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="I11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J11" t="s">
-        <v>210</v>
+        <v>211</v>
+      </c>
+      <c r="K11" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>365</v>
+        <v>344</v>
+      </c>
+      <c r="I12" t="s">
+        <v>210</v>
       </c>
       <c r="J12" t="s">
-        <v>260</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>259</v>
       </c>
       <c r="B13" t="s">
-        <v>349</v>
+        <v>365</v>
+      </c>
+      <c r="J13" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>350</v>
-      </c>
-      <c r="N14" t="s">
-        <v>429</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>351</v>
-      </c>
-      <c r="C15" t="s">
-        <v>184</v>
-      </c>
-      <c r="I15" t="s">
-        <v>198</v>
+        <v>350</v>
       </c>
       <c r="N15" t="s">
-        <v>198</v>
+        <v>429</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" t="s">
+        <v>351</v>
+      </c>
+      <c r="C16" t="s">
+        <v>184</v>
+      </c>
+      <c r="I16" t="s">
+        <v>198</v>
+      </c>
+      <c r="N16" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>226</v>
+      </c>
+      <c r="R16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>118</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>117</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>352</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I19" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="Q19" t="s">
+        <v>227</v>
+      </c>
+      <c r="R19" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>105</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>353</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J20" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="R20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>106</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>354</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K21" t="s">
         <v>275</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L21" t="s">
         <v>321</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N21" t="s">
         <v>430</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O21" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="P21" t="s">
+        <v>275</v>
+      </c>
+      <c r="R21" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>107</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>355</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J22" t="s">
         <v>248</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N22" t="s">
         <v>413</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O22" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="R22" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>108</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>109</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>357</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>176</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J24" t="s">
         <v>176</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M24" t="s">
         <v>410</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N24" t="s">
         <v>176</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O24" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="P24" t="s">
+        <v>491</v>
+      </c>
+      <c r="R24" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>110</v>
-      </c>
-      <c r="B24" t="s">
-        <v>358</v>
-      </c>
-      <c r="I24" t="s">
-        <v>207</v>
-      </c>
-      <c r="J24" t="s">
-        <v>236</v>
-      </c>
-      <c r="K24" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>253</v>
       </c>
       <c r="B25" t="s">
         <v>358</v>
       </c>
+      <c r="I25" t="s">
+        <v>207</v>
+      </c>
       <c r="J25" t="s">
+        <v>236</v>
+      </c>
+      <c r="K25" t="s">
+        <v>276</v>
+      </c>
+      <c r="P25" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>517</v>
+      </c>
+      <c r="R25" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>253</v>
+      </c>
+      <c r="B26" t="s">
+        <v>358</v>
+      </c>
+      <c r="J26" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>484</v>
+      </c>
+      <c r="B27" t="s">
+        <v>485</v>
+      </c>
+      <c r="P27" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J28" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>281</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>358</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K29" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>111</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>358</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K30" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>112</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>359</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I31" t="s">
         <v>231</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J31" t="s">
         <v>231</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K31" t="s">
         <v>231</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L31" t="s">
         <v>332</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N31" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="Q31" t="s">
+        <v>231</v>
+      </c>
+      <c r="R31" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>289</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>359</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K32" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>114</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>360</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>185</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H33" t="s">
         <v>198</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I33" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="Q33" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>113</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>360</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K34" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="R34" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>115</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="R35" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>521</v>
+      </c>
+      <c r="B36" t="s">
+        <v>522</v>
+      </c>
+      <c r="R36" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>116</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>362</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L37" t="s">
         <v>340</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M37" t="s">
         <v>400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>472</v>
+      </c>
+      <c r="B38" t="s">
+        <v>473</v>
+      </c>
+      <c r="P38" t="s">
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -2404,16 +2772,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B66207E-F3A7-4A76-96AD-A5712E9C1247}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2701,6 +3069,39 @@
       </c>
       <c r="C26" t="s">
         <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>477</v>
+      </c>
+      <c r="B27" t="s">
+        <v>368</v>
+      </c>
+      <c r="C27" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>475</v>
+      </c>
+      <c r="B28" t="s">
+        <v>368</v>
+      </c>
+      <c r="C28" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>479</v>
+      </c>
+      <c r="B29" t="s">
+        <v>368</v>
+      </c>
+      <c r="C29" t="s">
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -2711,11 +3112,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W117"/>
+  <dimension ref="A1:W124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q94" sqref="Q94"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2733,10 +3134,10 @@
     <col min="11" max="11" width="26.85546875" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="25.5703125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="31.5703125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="32" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="35.7109375" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="27.140625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="47.42578125" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="42.28515625" bestFit="1" customWidth="1"/>
@@ -2931,6 +3332,9 @@
       <c r="M4" t="s">
         <v>435</v>
       </c>
+      <c r="Q4" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2962,6 +3366,9 @@
       <c r="N6" t="s">
         <v>209</v>
       </c>
+      <c r="Q6" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2987,6 +3394,9 @@
       <c r="M8" t="s">
         <v>221</v>
       </c>
+      <c r="Q8" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -3036,6 +3446,9 @@
       <c r="K13" t="s">
         <v>341</v>
       </c>
+      <c r="Q13" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3061,1061 +3474,1306 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>489</v>
+      </c>
+      <c r="O17" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I18" t="s">
         <v>240</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J18" t="s">
         <v>291</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M18" t="s">
         <v>284</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N18" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="Q18" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>181</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J19" t="s">
         <v>240</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M19" t="s">
         <v>240</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N19" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>301</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J20" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" t="s">
         <v>210</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I22" t="s">
         <v>210</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J22" t="s">
         <v>210</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M22" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="O22" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>421</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M23" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>423</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M24" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H25" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="P25" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H26" t="s">
         <v>215</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J26" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="P26" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="O27" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>293</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J28" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>237</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I29" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="Q30" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>228</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J31" t="s">
         <v>228</v>
       </c>
-      <c r="M30" t="s">
+      <c r="M31" t="s">
         <v>228</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N31" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="O31" t="s">
+        <v>482</v>
+      </c>
+      <c r="P31" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>417</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M32" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>511</v>
+      </c>
+      <c r="P33" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>398</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L34" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M35" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>408</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L36" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I37" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M38" t="s">
         <v>416</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N38" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I39" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="Q39" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H40" t="s">
         <v>222</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J40" t="s">
         <v>222</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K40" t="s">
         <v>337</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M40" t="s">
         <v>415</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N40" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="P40" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="M39" t="s">
+      <c r="M41" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J42" t="s">
         <v>284</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K42" t="s">
         <v>222</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M42" t="s">
         <v>447</v>
       </c>
-      <c r="N40" t="s">
+      <c r="N42" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="O42" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>92</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G44" t="s">
         <v>92</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K44" t="s">
         <v>334</v>
       </c>
-      <c r="M42" t="s">
+      <c r="M44" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="Q44" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>438</v>
       </c>
-      <c r="M43" t="s">
+      <c r="M45" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>440</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M46" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>442</v>
       </c>
-      <c r="M45" t="s">
+      <c r="M47" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>44</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G48" t="s">
         <v>257</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J48" t="s">
         <v>268</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N48" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="P48" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>45</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H49" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>533</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>186</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B52" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>46</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B53" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>47</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H54" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="P54" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>48</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B55" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>49</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H56" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="P56" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>469</v>
+      </c>
+      <c r="O57" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>51</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J59" t="s">
         <v>318</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K59" t="s">
         <v>176</v>
       </c>
-      <c r="L54" t="s">
+      <c r="L59" t="s">
         <v>396</v>
       </c>
-      <c r="M54" t="s">
+      <c r="M59" t="s">
         <v>436</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N59" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="P59" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>459</v>
       </c>
-      <c r="N55" t="s">
+      <c r="N60" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>315</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J61" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>52</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K62" t="s">
         <v>325</v>
       </c>
-      <c r="N57" t="s">
+      <c r="N62" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="Q62" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>53</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H63" t="s">
         <v>212</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I63" t="s">
         <v>212</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J63" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="O63" t="s">
+        <v>503</v>
+      </c>
+      <c r="P63" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>271</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J64" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="P64" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>54</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H65" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="Q65" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>55</v>
       </c>
-      <c r="K61" t="s">
+      <c r="K66" t="s">
         <v>212</v>
       </c>
-      <c r="M61" t="s">
+      <c r="M66" t="s">
         <v>212</v>
       </c>
-      <c r="N61" t="s">
+      <c r="N66" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="O66" t="s">
+        <v>502</v>
+      </c>
+      <c r="P66" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>401</v>
       </c>
-      <c r="L62" t="s">
+      <c r="L67" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>56</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B68" t="s">
         <v>175</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G68" t="s">
         <v>195</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I68" t="s">
         <v>175</v>
       </c>
-      <c r="K63" t="s">
+      <c r="K68" t="s">
         <v>175</v>
       </c>
-      <c r="L63" t="s">
+      <c r="L68" t="s">
         <v>175</v>
       </c>
-      <c r="M63" t="s">
+      <c r="M68" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>57</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H69" t="s">
         <v>224</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J69" t="s">
         <v>266</v>
       </c>
-      <c r="M64" t="s">
+      <c r="M69" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="P69" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>58</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H70" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>59</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G71" t="s">
         <v>196</v>
       </c>
-      <c r="I66" t="s">
+      <c r="I71" t="s">
         <v>243</v>
       </c>
-      <c r="L66" t="s">
+      <c r="L71" t="s">
         <v>395</v>
       </c>
-      <c r="N66" t="s">
+      <c r="N71" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="O71" t="s">
+        <v>471</v>
+      </c>
+      <c r="P71" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>202</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G72" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>61</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H74" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="O74" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>245</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I75" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>319</v>
       </c>
-      <c r="J71" t="s">
+      <c r="J76" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>63</v>
       </c>
-      <c r="K73" t="s">
+      <c r="K78" t="s">
         <v>331</v>
       </c>
-      <c r="M73" t="s">
+      <c r="M78" t="s">
         <v>298</v>
       </c>
-      <c r="N73" t="s">
+      <c r="N78" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="O78" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>64</v>
       </c>
-      <c r="J74" t="s">
+      <c r="J79" t="s">
         <v>298</v>
       </c>
-      <c r="K74" t="s">
+      <c r="K79" t="s">
         <v>323</v>
       </c>
-      <c r="M74" t="s">
+      <c r="M79" t="s">
         <v>298</v>
       </c>
-      <c r="N74" t="s">
+      <c r="N79" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="O79" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>427</v>
       </c>
-      <c r="M75" t="s">
+      <c r="M80" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>65</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H81" t="s">
         <v>217</v>
       </c>
-      <c r="K76" t="s">
+      <c r="K81" t="s">
         <v>339</v>
       </c>
-      <c r="M76" t="s">
+      <c r="M81" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="P81" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>307</v>
       </c>
-      <c r="J77" t="s">
+      <c r="J82" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>66</v>
       </c>
-      <c r="J78" t="s">
+      <c r="J83" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>299</v>
       </c>
-      <c r="J79" t="s">
+      <c r="J84" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>67</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G85" t="s">
         <v>265</v>
       </c>
-      <c r="M80" t="s">
+      <c r="M85" t="s">
         <v>419</v>
       </c>
-      <c r="N80" t="s">
+      <c r="N85" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="Q85" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>311</v>
       </c>
-      <c r="J81" t="s">
+      <c r="J86" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>309</v>
       </c>
-      <c r="J82" t="s">
+      <c r="J87" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>305</v>
       </c>
-      <c r="J83" t="s">
+      <c r="J88" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>68</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B89" t="s">
         <v>183</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I89" t="s">
         <v>247</v>
       </c>
-      <c r="N84" t="s">
+      <c r="N89" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>69</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H90" t="s">
         <v>233</v>
       </c>
-      <c r="J85" t="s">
+      <c r="J90" t="s">
         <v>278</v>
       </c>
-      <c r="K85" t="s">
+      <c r="K90" t="s">
         <v>328</v>
       </c>
-      <c r="M85" t="s">
+      <c r="M90" t="s">
         <v>444</v>
       </c>
-      <c r="N85" t="s">
+      <c r="N90" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="P90" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>70</v>
       </c>
-      <c r="L86" t="s">
+      <c r="L91" t="s">
         <v>263</v>
       </c>
-      <c r="M86" t="s">
+      <c r="M91" t="s">
         <v>411</v>
       </c>
-      <c r="N86" t="s">
+      <c r="N91" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>71</v>
       </c>
-      <c r="J87" t="s">
+      <c r="J92" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>72</v>
       </c>
-      <c r="J88" t="s">
+      <c r="J93" t="s">
         <v>314</v>
       </c>
-      <c r="N88" t="s">
+      <c r="N93" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>73</v>
       </c>
-      <c r="H89" t="s">
+      <c r="H94" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>74</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B95" t="s">
         <v>173</v>
       </c>
-      <c r="I90" t="s">
+      <c r="I95" t="s">
         <v>252</v>
       </c>
-      <c r="J90" t="s">
+      <c r="J95" t="s">
         <v>277</v>
       </c>
-      <c r="K90" t="s">
+      <c r="K95" t="s">
         <v>336</v>
       </c>
-      <c r="M90" t="s">
+      <c r="M95" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="Q95" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>269</v>
       </c>
-      <c r="J91" t="s">
+      <c r="J96" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>496</v>
+      </c>
+      <c r="O97" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>498</v>
+      </c>
+      <c r="O98" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>303</v>
       </c>
-      <c r="J92" t="s">
+      <c r="J99" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>219</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H100" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>75</v>
       </c>
-      <c r="J94" t="s">
+      <c r="J101" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="Q101" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>76</v>
       </c>
-      <c r="H95" t="s">
+      <c r="H102" t="s">
         <v>232</v>
       </c>
-      <c r="K95" t="s">
+      <c r="K102" t="s">
         <v>342</v>
       </c>
-      <c r="L95" t="s">
+      <c r="L102" t="s">
         <v>342</v>
       </c>
-      <c r="N95" t="s">
+      <c r="N102" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="O102" t="s">
+        <v>494</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>77</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G103" t="s">
         <v>197</v>
       </c>
-      <c r="H96" t="s">
+      <c r="H103" t="s">
         <v>224</v>
       </c>
-      <c r="I96" t="s">
+      <c r="I103" t="s">
         <v>239</v>
       </c>
-      <c r="J96" t="s">
+      <c r="J103" t="s">
         <v>239</v>
       </c>
-      <c r="K96" t="s">
+      <c r="K103" t="s">
         <v>324</v>
       </c>
-      <c r="L96" t="s">
+      <c r="L103" t="s">
         <v>407</v>
       </c>
-      <c r="N96" t="s">
+      <c r="N103" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="O103" t="s">
+        <v>495</v>
+      </c>
+      <c r="P103" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>78</v>
       </c>
-      <c r="H97" t="s">
+      <c r="H104" t="s">
         <v>216</v>
       </c>
-      <c r="J97" t="s">
+      <c r="J104" t="s">
         <v>286</v>
       </c>
-      <c r="K97" t="s">
+      <c r="K104" t="s">
         <v>338</v>
       </c>
-      <c r="L97" t="s">
+      <c r="L104" t="s">
         <v>216</v>
       </c>
-      <c r="M97" t="s">
+      <c r="M104" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="P104" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>80</v>
       </c>
-      <c r="J99" t="s">
+      <c r="J106" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="Q106" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>81</v>
       </c>
-      <c r="K100" t="s">
+      <c r="K107" t="s">
         <v>329</v>
       </c>
-      <c r="M100" t="s">
+      <c r="M107" t="s">
         <v>412</v>
       </c>
-      <c r="N100" t="s">
+      <c r="N107" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="Q107" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>261</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G108" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>82</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B109" t="s">
         <v>182</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H109" t="s">
         <v>225</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I109" t="s">
         <v>182</v>
       </c>
-      <c r="J102" t="s">
+      <c r="J109" t="s">
         <v>225</v>
       </c>
-      <c r="K102" t="s">
+      <c r="K109" t="s">
         <v>322</v>
       </c>
-      <c r="M102" t="s">
+      <c r="M109" t="s">
         <v>182</v>
       </c>
-      <c r="N102" t="s">
+      <c r="N109" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="P109" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>83</v>
       </c>
-      <c r="H103" t="s">
+      <c r="H110" t="s">
         <v>216</v>
       </c>
-      <c r="I103" t="s">
+      <c r="I110" t="s">
         <v>242</v>
       </c>
-      <c r="J103" t="s">
+      <c r="J110" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="P110" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>84</v>
       </c>
-      <c r="J104" t="s">
+      <c r="J111" t="s">
         <v>267</v>
       </c>
-      <c r="M104" t="s">
+      <c r="M111" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="Q111" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>279</v>
       </c>
-      <c r="J109" t="s">
+      <c r="J116" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="O116" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>177</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B117" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="O117" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>193</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G118" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="Q119" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>466</v>
       </c>
-      <c r="N113" t="s">
+      <c r="N120" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>178</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B121" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>464</v>
       </c>
-      <c r="N115" t="s">
+      <c r="N122" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>90</v>
       </c>
-      <c r="H116" t="s">
+      <c r="H123" t="s">
         <v>218</v>
       </c>
-      <c r="K116" t="s">
+      <c r="K123" t="s">
         <v>333</v>
       </c>
-      <c r="M116" t="s">
+      <c r="M123" t="s">
         <v>218</v>
       </c>
-      <c r="N116" t="s">
+      <c r="N123" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="Q123" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>91</v>
       </c>
-      <c r="N117" t="s">
+      <c r="N124" t="s">
         <v>222</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code and two courses to glossary
</commit_message>
<xml_diff>
--- a/book/glossary/Glossary_CT.xlsx
+++ b/book/glossary/Glossary_CT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\werel\Documents\P-RE-CONNECT\ECT_Book\book\glossary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D9A108-DD40-4ABB-AF93-891359D5D866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BB37B0-E983-48B2-9F82-92D988D1C864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="621">
   <si>
     <t>Symbol</t>
   </si>
@@ -1603,12 +1603,6 @@
     <t>Partial factor</t>
   </si>
   <si>
-    <t>$\Psi$</t>
-  </si>
-  <si>
-    <t>Psi</t>
-  </si>
-  <si>
     <t>Combination factor</t>
   </si>
   <si>
@@ -1694,6 +1688,219 @@
   </si>
   <si>
     <t>Ratio between $F_k$ and $F$, relative normal force</t>
+  </si>
+  <si>
+    <t>Rotational inertia</t>
+  </si>
+  <si>
+    <t>Lagrangian</t>
+  </si>
+  <si>
+    <t>$\dot{u}$</t>
+  </si>
+  <si>
+    <t>$\omega_0$</t>
+  </si>
+  <si>
+    <t>Natural frequency</t>
+  </si>
+  <si>
+    <t>$T_0$</t>
+  </si>
+  <si>
+    <t>Natural period</t>
+  </si>
+  <si>
+    <t>$\varphi_0$</t>
+  </si>
+  <si>
+    <t>Natural phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>$a_n$</t>
+  </si>
+  <si>
+    <t>$b_n$</t>
+  </si>
+  <si>
+    <t>Damping ratio</t>
+  </si>
+  <si>
+    <t>$\ddot{u}$</t>
+  </si>
+  <si>
+    <t>$\vec{u}$</t>
+  </si>
+  <si>
+    <t>Displacement vector</t>
+  </si>
+  <si>
+    <t>$\vec{f}$</t>
+  </si>
+  <si>
+    <t>Force vector</t>
+  </si>
+  <si>
+    <t>$\mathbf{M}$</t>
+  </si>
+  <si>
+    <t>Mass matrix</t>
+  </si>
+  <si>
+    <t>$\mathbf{K}$</t>
+  </si>
+  <si>
+    <t>Stiffness matrix</t>
+  </si>
+  <si>
+    <t>Amplitude, area</t>
+  </si>
+  <si>
+    <t>Heaviside step function, water level</t>
+  </si>
+  <si>
+    <t>Water elevation</t>
+  </si>
+  <si>
+    <t>Moment, inertia of the water</t>
+  </si>
+  <si>
+    <t>Loss factor</t>
+  </si>
+  <si>
+    <t>Cross sectional area</t>
+  </si>
+  <si>
+    <t>$C_u$</t>
+  </si>
+  <si>
+    <t>Uniformity coefficient</t>
+  </si>
+  <si>
+    <t>Silt</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Organic</t>
+  </si>
+  <si>
+    <t>Poorly graded</t>
+  </si>
+  <si>
+    <t>$P_t$</t>
+  </si>
+  <si>
+    <t>Peat</t>
+  </si>
+  <si>
+    <t>Void ratio</t>
+  </si>
+  <si>
+    <t>$RD$</t>
+  </si>
+  <si>
+    <t>Total stress</t>
+  </si>
+  <si>
+    <t>Effective stress</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Dynamic viscosity</t>
+  </si>
+  <si>
+    <t>Intrinsic permeability</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>Hydraulic conductivity</t>
+  </si>
+  <si>
+    <t>Seepage force</t>
+  </si>
+  <si>
+    <t>Hydraulic gradient</t>
+  </si>
+  <si>
+    <t>Diameter, depth</t>
+  </si>
+  <si>
+    <t>$\psi$</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>Stream function</t>
+  </si>
+  <si>
+    <t>Thickness of flow plane</t>
+  </si>
+  <si>
+    <t>Porosity, length perpendicular to flow</t>
+  </si>
+  <si>
+    <t>Length in direction of flow</t>
+  </si>
+  <si>
+    <t>Radius of pumped area</t>
+  </si>
+  <si>
+    <t>High plasticity, height</t>
+  </si>
+  <si>
+    <t>Gravel, shear modulus</t>
+  </si>
+  <si>
+    <t>$m_v$</t>
+  </si>
+  <si>
+    <t>Compressibility coefficient</t>
+  </si>
+  <si>
+    <t>$c_v$</t>
+  </si>
+  <si>
+    <t>Consolidation coefficient</t>
+  </si>
+  <si>
+    <t>Radius of footing</t>
+  </si>
+  <si>
+    <t>Compression constant, cohesion</t>
+  </si>
+  <si>
+    <t>Potential, friction angle</t>
+  </si>
+  <si>
+    <t>Pore water pressure, bearing capacity</t>
+  </si>
+  <si>
+    <t>Sand, degree of saturation, shape factor</t>
+  </si>
+  <si>
+    <t>Low plasticity, length</t>
+  </si>
+  <si>
+    <t>Bulk modulus, coefficient of lateral earth pressure</t>
+  </si>
+  <si>
+    <t>Specific discharge, pressure</t>
+  </si>
+  <si>
+    <t>Well graded, weight</t>
+  </si>
+  <si>
+    <t>Discharge, earth pressure</t>
   </si>
 </sst>
 </file>
@@ -2022,12 +2229,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2617A03-EA22-4211-801A-355FACE4DDAC}">
-  <dimension ref="A1:X38"/>
+  <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="U20" sqref="U20"/>
+      <selection pane="bottomLeft" activeCell="V44" sqref="V44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,8 +2257,8 @@
     <col min="16" max="16" width="24" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="28.42578125" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="31.28515625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -2248,7 +2455,7 @@
         <v>508</v>
       </c>
       <c r="R4" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -2290,6 +2497,9 @@
       <c r="R6" t="s">
         <v>520</v>
       </c>
+      <c r="T6" t="s">
+        <v>590</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2318,6 +2528,9 @@
       <c r="R8" t="s">
         <v>216</v>
       </c>
+      <c r="S8" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2360,6 +2573,9 @@
       <c r="Q11" t="s">
         <v>211</v>
       </c>
+      <c r="T11" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2393,6 +2609,9 @@
       <c r="B14" t="s">
         <v>349</v>
       </c>
+      <c r="S14" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2427,8 +2646,11 @@
       <c r="R16" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>118</v>
       </c>
@@ -2436,7 +2658,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -2444,7 +2666,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -2460,8 +2682,11 @@
       <c r="R19" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T19" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -2472,10 +2697,10 @@
         <v>258</v>
       </c>
       <c r="R20" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -2500,8 +2725,11 @@
       <c r="R21" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T21" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>107</v>
       </c>
@@ -2520,8 +2748,11 @@
       <c r="R22" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T22" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -2529,7 +2760,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>109</v>
       </c>
@@ -2555,10 +2786,16 @@
         <v>491</v>
       </c>
       <c r="R24" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+      <c r="S24" t="s">
+        <v>176</v>
+      </c>
+      <c r="T24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>110</v>
       </c>
@@ -2581,10 +2818,13 @@
         <v>517</v>
       </c>
       <c r="R25" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+        <v>533</v>
+      </c>
+      <c r="T25" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>253</v>
       </c>
@@ -2594,8 +2834,11 @@
       <c r="J26" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T26" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>484</v>
       </c>
@@ -2606,7 +2849,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>255</v>
       </c>
@@ -2617,7 +2860,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>281</v>
       </c>
@@ -2628,7 +2871,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -2639,7 +2882,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>112</v>
       </c>
@@ -2667,8 +2910,11 @@
       <c r="R31" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T31" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>289</v>
       </c>
@@ -2678,8 +2924,11 @@
       <c r="K32" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T32" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -2699,64 +2948,95 @@
         <v>226</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>557</v>
       </c>
       <c r="B34" t="s">
         <v>360</v>
       </c>
-      <c r="K34" t="s">
+      <c r="S34" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" t="s">
+        <v>360</v>
+      </c>
+      <c r="K35" t="s">
         <v>288</v>
       </c>
-      <c r="R34" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="R35" t="s">
+        <v>541</v>
+      </c>
+      <c r="T35" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>115</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>361</v>
       </c>
-      <c r="R35" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="R36" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>598</v>
+      </c>
+      <c r="B37" t="s">
+        <v>599</v>
+      </c>
+      <c r="R37" t="s">
         <v>521</v>
       </c>
-      <c r="B36" t="s">
-        <v>522</v>
-      </c>
-      <c r="R36" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="T37" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>116</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>362</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L38" t="s">
         <v>340</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M38" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="S38" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>553</v>
+      </c>
+      <c r="B39" t="s">
+        <v>362</v>
+      </c>
+      <c r="S39" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>472</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>473</v>
       </c>
-      <c r="P38" t="s">
+      <c r="P40" t="s">
         <v>474</v>
       </c>
     </row>
@@ -2775,7 +3055,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3112,11 +3392,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W124"/>
+  <dimension ref="A1:W138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q1:Q1048576"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S2" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3138,8 +3418,8 @@
     <col min="15" max="15" width="35.7109375" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="27.140625" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="47.42578125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.5703125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="46.5703125" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -3333,7 +3613,13 @@
         <v>435</v>
       </c>
       <c r="Q4" t="s">
-        <v>526</v>
+        <v>524</v>
+      </c>
+      <c r="R4" t="s">
+        <v>335</v>
+      </c>
+      <c r="S4" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -3346,1433 +3632,1707 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>190</v>
-      </c>
-      <c r="H6" t="s">
-        <v>209</v>
-      </c>
-      <c r="I6" t="s">
-        <v>244</v>
-      </c>
-      <c r="J6" t="s">
-        <v>209</v>
-      </c>
-      <c r="K6" t="s">
-        <v>330</v>
-      </c>
-      <c r="N6" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>525</v>
+        <v>560</v>
+      </c>
+      <c r="R6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>199</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>200</v>
+        <v>190</v>
+      </c>
+      <c r="H7" t="s">
+        <v>209</v>
+      </c>
+      <c r="I7" t="s">
+        <v>244</v>
+      </c>
+      <c r="J7" t="s">
+        <v>209</v>
+      </c>
+      <c r="K7" t="s">
+        <v>330</v>
+      </c>
+      <c r="N7" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>523</v>
+      </c>
+      <c r="R7" t="s">
+        <v>572</v>
+      </c>
+      <c r="S7" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
       <c r="G8" t="s">
-        <v>264</v>
-      </c>
-      <c r="H8" t="s">
-        <v>221</v>
-      </c>
-      <c r="J8" t="s">
-        <v>221</v>
-      </c>
-      <c r="M8" t="s">
-        <v>221</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>192</v>
+        <v>264</v>
+      </c>
+      <c r="H9" t="s">
+        <v>221</v>
+      </c>
+      <c r="J9" t="s">
+        <v>221</v>
+      </c>
+      <c r="M9" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>406</v>
-      </c>
-      <c r="L10" t="s">
-        <v>405</v>
+        <v>191</v>
+      </c>
+      <c r="G10" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>326</v>
-      </c>
-      <c r="K11" t="s">
-        <v>327</v>
-      </c>
-      <c r="N11" t="s">
-        <v>221</v>
+        <v>406</v>
+      </c>
+      <c r="L11" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>296</v>
-      </c>
-      <c r="J12" t="s">
-        <v>297</v>
+        <v>561</v>
+      </c>
+      <c r="R12" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>119</v>
-      </c>
-      <c r="J13" t="s">
-        <v>287</v>
+        <v>326</v>
       </c>
       <c r="K13" t="s">
-        <v>341</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>541</v>
+        <v>327</v>
+      </c>
+      <c r="N13" t="s">
+        <v>221</v>
+      </c>
+      <c r="R13" t="s">
+        <v>577</v>
+      </c>
+      <c r="S13" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>455</v>
-      </c>
-      <c r="N14" t="s">
-        <v>456</v>
+        <v>296</v>
+      </c>
+      <c r="J14" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="N15" t="s">
-        <v>450</v>
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="J15" t="s">
+        <v>287</v>
+      </c>
+      <c r="K15" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>539</v>
+      </c>
+      <c r="S15" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>455</v>
+      </c>
+      <c r="N16" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>609</v>
+      </c>
+      <c r="S17" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" t="s">
+        <v>450</v>
+      </c>
+      <c r="S18" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>578</v>
+      </c>
+      <c r="S19" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>201</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G20" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>489</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O21" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I22" t="s">
         <v>240</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J22" t="s">
         <v>291</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M22" t="s">
         <v>284</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N22" t="s">
         <v>284</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="Q22" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
+      </c>
+      <c r="J23" t="s">
+        <v>240</v>
+      </c>
+      <c r="M23" t="s">
+        <v>240</v>
+      </c>
+      <c r="N23" t="s">
+        <v>461</v>
+      </c>
+      <c r="S23" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>301</v>
+      </c>
+      <c r="J24" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" t="s">
+        <v>229</v>
+      </c>
+      <c r="S25" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I26" t="s">
+        <v>210</v>
+      </c>
+      <c r="J26" t="s">
+        <v>210</v>
+      </c>
+      <c r="M26" t="s">
+        <v>434</v>
+      </c>
+      <c r="O26" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>525</v>
+      </c>
+      <c r="R26" t="s">
+        <v>434</v>
+      </c>
+      <c r="S26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>421</v>
+      </c>
+      <c r="M27" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>423</v>
+      </c>
+      <c r="M28" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" t="s">
+        <v>214</v>
+      </c>
+      <c r="P29" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" t="s">
+        <v>215</v>
+      </c>
+      <c r="J30" t="s">
+        <v>215</v>
+      </c>
+      <c r="P30" t="s">
+        <v>215</v>
+      </c>
+      <c r="R30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>174</v>
+      </c>
+      <c r="O31" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>527</v>
+      </c>
+      <c r="S31" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>566</v>
+      </c>
+      <c r="R32" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>293</v>
+      </c>
+      <c r="J33" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>237</v>
+      </c>
+      <c r="I34" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" t="s">
+        <v>228</v>
+      </c>
+      <c r="J36" t="s">
+        <v>228</v>
+      </c>
+      <c r="M36" t="s">
+        <v>228</v>
+      </c>
+      <c r="N36" t="s">
+        <v>228</v>
+      </c>
+      <c r="O36" t="s">
+        <v>482</v>
+      </c>
+      <c r="P36" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>228</v>
+      </c>
+      <c r="R36" t="s">
+        <v>228</v>
+      </c>
+      <c r="S36" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>417</v>
+      </c>
+      <c r="M37" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>511</v>
+      </c>
+      <c r="P38" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>398</v>
+      </c>
+      <c r="L39" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="M40" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>408</v>
+      </c>
+      <c r="L41" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="I42" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="M43" t="s">
+        <v>416</v>
+      </c>
+      <c r="N43" t="s">
+        <v>416</v>
+      </c>
+      <c r="R43" t="s">
+        <v>416</v>
+      </c>
+      <c r="S43" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="I44" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>528</v>
+      </c>
+      <c r="S44" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="H45" t="s">
+        <v>222</v>
+      </c>
+      <c r="J45" t="s">
+        <v>222</v>
+      </c>
+      <c r="K45" t="s">
+        <v>337</v>
+      </c>
+      <c r="M45" t="s">
+        <v>415</v>
+      </c>
+      <c r="N45" t="s">
+        <v>454</v>
+      </c>
+      <c r="P45" t="s">
+        <v>222</v>
+      </c>
+      <c r="R45" t="s">
+        <v>574</v>
+      </c>
+      <c r="S45" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="M46" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="J47" t="s">
+        <v>284</v>
+      </c>
+      <c r="K47" t="s">
+        <v>222</v>
+      </c>
+      <c r="M47" t="s">
+        <v>447</v>
+      </c>
+      <c r="N47" t="s">
+        <v>457</v>
+      </c>
+      <c r="O47" t="s">
+        <v>501</v>
+      </c>
+      <c r="R47" t="s">
+        <v>573</v>
+      </c>
+      <c r="S47" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" t="s">
+        <v>92</v>
+      </c>
+      <c r="G49" t="s">
+        <v>92</v>
+      </c>
+      <c r="K49" t="s">
+        <v>334</v>
+      </c>
+      <c r="M49" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>535</v>
+      </c>
+      <c r="R49" t="s">
+        <v>92</v>
+      </c>
+      <c r="S49" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>438</v>
+      </c>
+      <c r="M50" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>440</v>
+      </c>
+      <c r="M51" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>442</v>
+      </c>
+      <c r="M52" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="G53" t="s">
+        <v>257</v>
+      </c>
+      <c r="J53" t="s">
+        <v>268</v>
+      </c>
+      <c r="N53" t="s">
+        <v>339</v>
+      </c>
+      <c r="P53" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>45</v>
+      </c>
+      <c r="H54" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>47</v>
+      </c>
+      <c r="H59" t="s">
+        <v>223</v>
+      </c>
+      <c r="P59" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>48</v>
+      </c>
+      <c r="B60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>49</v>
+      </c>
+      <c r="H61" t="s">
+        <v>188</v>
+      </c>
+      <c r="P61" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>469</v>
+      </c>
+      <c r="O62" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>50</v>
+      </c>
+      <c r="R63" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>51</v>
+      </c>
+      <c r="J64" t="s">
+        <v>318</v>
+      </c>
+      <c r="K64" t="s">
+        <v>176</v>
+      </c>
+      <c r="L64" t="s">
+        <v>396</v>
+      </c>
+      <c r="M64" t="s">
+        <v>436</v>
+      </c>
+      <c r="N64" t="s">
+        <v>453</v>
+      </c>
+      <c r="P64" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>543</v>
+      </c>
+      <c r="R64" t="s">
+        <v>396</v>
+      </c>
+      <c r="S64" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>459</v>
+      </c>
+      <c r="N65" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>315</v>
+      </c>
+      <c r="J66" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>52</v>
+      </c>
+      <c r="K67" t="s">
+        <v>325</v>
+      </c>
+      <c r="N67" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>426</v>
+      </c>
+      <c r="R67" t="s">
+        <v>422</v>
+      </c>
+      <c r="S67" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>570</v>
+      </c>
+      <c r="R68" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>53</v>
+      </c>
+      <c r="H69" t="s">
+        <v>212</v>
+      </c>
+      <c r="I69" t="s">
+        <v>212</v>
+      </c>
+      <c r="J69" t="s">
+        <v>212</v>
+      </c>
+      <c r="O69" t="s">
+        <v>503</v>
+      </c>
+      <c r="P69" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>212</v>
+      </c>
+      <c r="R69" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>271</v>
+      </c>
+      <c r="J70" t="s">
+        <v>272</v>
+      </c>
+      <c r="P70" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>54</v>
+      </c>
+      <c r="H71" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>55</v>
+      </c>
+      <c r="K72" t="s">
+        <v>212</v>
+      </c>
+      <c r="M72" t="s">
+        <v>212</v>
+      </c>
+      <c r="N72" t="s">
+        <v>212</v>
+      </c>
+      <c r="O72" t="s">
+        <v>502</v>
+      </c>
+      <c r="P72" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>212</v>
+      </c>
+      <c r="S72" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>401</v>
+      </c>
+      <c r="L73" t="s">
+        <v>402</v>
+      </c>
+      <c r="R73" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>56</v>
+      </c>
+      <c r="B74" t="s">
+        <v>175</v>
+      </c>
+      <c r="G74" t="s">
+        <v>195</v>
+      </c>
+      <c r="I74" t="s">
+        <v>175</v>
+      </c>
+      <c r="K74" t="s">
+        <v>175</v>
+      </c>
+      <c r="L74" t="s">
+        <v>175</v>
+      </c>
+      <c r="M74" t="s">
+        <v>175</v>
+      </c>
+      <c r="R74" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>607</v>
+      </c>
+      <c r="S75" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>57</v>
+      </c>
+      <c r="H76" t="s">
+        <v>224</v>
+      </c>
+      <c r="J76" t="s">
+        <v>266</v>
+      </c>
+      <c r="M76" t="s">
+        <v>445</v>
+      </c>
+      <c r="P76" t="s">
+        <v>266</v>
+      </c>
+      <c r="R76" t="s">
+        <v>575</v>
+      </c>
+      <c r="S76" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>568</v>
+      </c>
+      <c r="R77" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>58</v>
+      </c>
+      <c r="H78" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>59</v>
+      </c>
+      <c r="G79" t="s">
+        <v>196</v>
+      </c>
+      <c r="I79" t="s">
+        <v>243</v>
+      </c>
+      <c r="L79" t="s">
+        <v>395</v>
+      </c>
+      <c r="N79" t="s">
+        <v>452</v>
+      </c>
+      <c r="O79" t="s">
+        <v>471</v>
+      </c>
+      <c r="P79" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>549</v>
+      </c>
+      <c r="S79" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>202</v>
+      </c>
+      <c r="G80" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>61</v>
+      </c>
+      <c r="H82" t="s">
+        <v>208</v>
+      </c>
+      <c r="O82" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>245</v>
+      </c>
+      <c r="I83" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>319</v>
+      </c>
+      <c r="J84" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>62</v>
+      </c>
+      <c r="S85" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>63</v>
+      </c>
+      <c r="K86" t="s">
+        <v>331</v>
+      </c>
+      <c r="M86" t="s">
+        <v>298</v>
+      </c>
+      <c r="N86" t="s">
+        <v>298</v>
+      </c>
+      <c r="O86" t="s">
+        <v>323</v>
+      </c>
+      <c r="S86" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>64</v>
+      </c>
+      <c r="J87" t="s">
+        <v>298</v>
+      </c>
+      <c r="K87" t="s">
+        <v>323</v>
+      </c>
+      <c r="M87" t="s">
+        <v>298</v>
+      </c>
+      <c r="N87" t="s">
+        <v>298</v>
+      </c>
+      <c r="O87" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>323</v>
+      </c>
+      <c r="R87" t="s">
+        <v>424</v>
+      </c>
+      <c r="S87" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>584</v>
+      </c>
+      <c r="S88" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>427</v>
+      </c>
+      <c r="M89" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>65</v>
+      </c>
+      <c r="H90" t="s">
+        <v>217</v>
+      </c>
+      <c r="K90" t="s">
+        <v>339</v>
+      </c>
+      <c r="M90" t="s">
+        <v>433</v>
+      </c>
+      <c r="P90" t="s">
+        <v>504</v>
+      </c>
+      <c r="S90" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>307</v>
+      </c>
+      <c r="J91" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>66</v>
+      </c>
+      <c r="J92" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>299</v>
+      </c>
+      <c r="J93" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>67</v>
+      </c>
+      <c r="G94" t="s">
+        <v>265</v>
+      </c>
+      <c r="M94" t="s">
+        <v>419</v>
+      </c>
+      <c r="N94" t="s">
+        <v>419</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>522</v>
+      </c>
+      <c r="R94" t="s">
+        <v>419</v>
+      </c>
+      <c r="S94" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>311</v>
+      </c>
+      <c r="J95" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>309</v>
+      </c>
+      <c r="J96" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>305</v>
+      </c>
+      <c r="J97" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>68</v>
+      </c>
+      <c r="B98" t="s">
+        <v>183</v>
+      </c>
+      <c r="I98" t="s">
+        <v>247</v>
+      </c>
+      <c r="N98" t="s">
+        <v>468</v>
+      </c>
+      <c r="S98" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>69</v>
+      </c>
+      <c r="H99" t="s">
+        <v>233</v>
+      </c>
+      <c r="J99" t="s">
+        <v>278</v>
+      </c>
+      <c r="K99" t="s">
+        <v>328</v>
+      </c>
+      <c r="M99" t="s">
+        <v>444</v>
+      </c>
+      <c r="N99" t="s">
+        <v>449</v>
+      </c>
+      <c r="P99" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>278</v>
+      </c>
+      <c r="S99" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>587</v>
+      </c>
+      <c r="S100" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>70</v>
+      </c>
+      <c r="L101" t="s">
+        <v>263</v>
+      </c>
+      <c r="M101" t="s">
+        <v>411</v>
+      </c>
+      <c r="N101" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>71</v>
+      </c>
+      <c r="J102" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>72</v>
+      </c>
+      <c r="J103" t="s">
+        <v>314</v>
+      </c>
+      <c r="N103" t="s">
+        <v>462</v>
+      </c>
+      <c r="S103" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>73</v>
+      </c>
+      <c r="H104" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>74</v>
+      </c>
+      <c r="B105" t="s">
+        <v>173</v>
+      </c>
+      <c r="I105" t="s">
+        <v>252</v>
+      </c>
+      <c r="J105" t="s">
+        <v>277</v>
+      </c>
+      <c r="K105" t="s">
+        <v>336</v>
+      </c>
+      <c r="M105" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>536</v>
+      </c>
+      <c r="S105" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>269</v>
+      </c>
+      <c r="J106" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>496</v>
+      </c>
+      <c r="O107" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>498</v>
+      </c>
+      <c r="O108" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>303</v>
+      </c>
+      <c r="J109" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>219</v>
+      </c>
+      <c r="H110" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>75</v>
+      </c>
+      <c r="J111" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>76</v>
+      </c>
+      <c r="H112" t="s">
+        <v>232</v>
+      </c>
+      <c r="K112" t="s">
+        <v>342</v>
+      </c>
+      <c r="L112" t="s">
+        <v>342</v>
+      </c>
+      <c r="N112" t="s">
+        <v>342</v>
+      </c>
+      <c r="O112" t="s">
+        <v>494</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>232</v>
+      </c>
+      <c r="R112" t="s">
+        <v>342</v>
+      </c>
+      <c r="S112" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>77</v>
+      </c>
+      <c r="G113" t="s">
+        <v>197</v>
+      </c>
+      <c r="H113" t="s">
+        <v>224</v>
+      </c>
+      <c r="I113" t="s">
+        <v>239</v>
+      </c>
+      <c r="J113" t="s">
+        <v>239</v>
+      </c>
+      <c r="K113" t="s">
+        <v>324</v>
+      </c>
+      <c r="L113" t="s">
+        <v>407</v>
+      </c>
+      <c r="N113" t="s">
+        <v>458</v>
+      </c>
+      <c r="O113" t="s">
+        <v>495</v>
+      </c>
+      <c r="P113" t="s">
+        <v>509</v>
+      </c>
+      <c r="R113" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>555</v>
+      </c>
+      <c r="R114" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>78</v>
+      </c>
+      <c r="H115" t="s">
+        <v>216</v>
+      </c>
+      <c r="J115" t="s">
+        <v>286</v>
+      </c>
+      <c r="K115" t="s">
+        <v>338</v>
+      </c>
+      <c r="L115" t="s">
+        <v>216</v>
+      </c>
+      <c r="M115" t="s">
+        <v>432</v>
+      </c>
+      <c r="P115" t="s">
+        <v>216</v>
+      </c>
+      <c r="R115" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>564</v>
+      </c>
+      <c r="R117" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>552</v>
+      </c>
+      <c r="R118" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>563</v>
+      </c>
+      <c r="R119" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>80</v>
+      </c>
+      <c r="J120" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>81</v>
+      </c>
+      <c r="K121" t="s">
+        <v>329</v>
+      </c>
+      <c r="M121" t="s">
+        <v>412</v>
+      </c>
+      <c r="N121" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>261</v>
+      </c>
+      <c r="G122" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>82</v>
+      </c>
+      <c r="B123" t="s">
+        <v>182</v>
+      </c>
+      <c r="H123" t="s">
+        <v>225</v>
+      </c>
+      <c r="I123" t="s">
+        <v>182</v>
+      </c>
+      <c r="J123" t="s">
+        <v>225</v>
+      </c>
+      <c r="K123" t="s">
+        <v>322</v>
+      </c>
+      <c r="M123" t="s">
+        <v>182</v>
+      </c>
+      <c r="N123" t="s">
+        <v>182</v>
+      </c>
+      <c r="P123" t="s">
+        <v>225</v>
+      </c>
+      <c r="S123" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>83</v>
+      </c>
+      <c r="H124" t="s">
+        <v>216</v>
+      </c>
+      <c r="I124" t="s">
+        <v>242</v>
+      </c>
+      <c r="J124" t="s">
+        <v>216</v>
+      </c>
+      <c r="P124" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>84</v>
+      </c>
+      <c r="J125" t="s">
+        <v>267</v>
+      </c>
+      <c r="M125" t="s">
+        <v>420</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>534</v>
+      </c>
+      <c r="R125" t="s">
+        <v>576</v>
+      </c>
+      <c r="S125" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>279</v>
+      </c>
+      <c r="J130" t="s">
+        <v>280</v>
+      </c>
+      <c r="O130" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>177</v>
+      </c>
+      <c r="B131" t="s">
+        <v>179</v>
+      </c>
+      <c r="O131" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>193</v>
+      </c>
+      <c r="G132" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q133" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>181</v>
-      </c>
-      <c r="J19" t="s">
-        <v>240</v>
-      </c>
-      <c r="M19" t="s">
-        <v>240</v>
-      </c>
-      <c r="N19" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>301</v>
-      </c>
-      <c r="J20" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" t="s">
-        <v>210</v>
-      </c>
-      <c r="I22" t="s">
-        <v>210</v>
-      </c>
-      <c r="J22" t="s">
-        <v>210</v>
-      </c>
-      <c r="M22" t="s">
-        <v>434</v>
-      </c>
-      <c r="O22" t="s">
-        <v>488</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>421</v>
-      </c>
-      <c r="M23" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>423</v>
-      </c>
-      <c r="M24" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" t="s">
-        <v>214</v>
-      </c>
-      <c r="P25" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" t="s">
-        <v>215</v>
-      </c>
-      <c r="J26" t="s">
-        <v>215</v>
-      </c>
-      <c r="P26" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="s">
-        <v>174</v>
-      </c>
-      <c r="O27" t="s">
-        <v>481</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>293</v>
-      </c>
-      <c r="J28" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>237</v>
-      </c>
-      <c r="I29" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="H31" t="s">
-        <v>228</v>
-      </c>
-      <c r="J31" t="s">
-        <v>228</v>
-      </c>
-      <c r="M31" t="s">
-        <v>228</v>
-      </c>
-      <c r="N31" t="s">
-        <v>228</v>
-      </c>
-      <c r="O31" t="s">
-        <v>482</v>
-      </c>
-      <c r="P31" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>417</v>
-      </c>
-      <c r="M32" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>511</v>
-      </c>
-      <c r="P33" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>398</v>
-      </c>
-      <c r="L34" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="M35" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>408</v>
-      </c>
-      <c r="L36" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-      <c r="I37" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="M38" t="s">
-        <v>416</v>
-      </c>
-      <c r="N38" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-      <c r="I39" t="s">
-        <v>249</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-      <c r="H40" t="s">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>466</v>
+      </c>
+      <c r="N134" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>178</v>
+      </c>
+      <c r="B135" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>464</v>
+      </c>
+      <c r="N136" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>90</v>
+      </c>
+      <c r="H137" t="s">
+        <v>218</v>
+      </c>
+      <c r="K137" t="s">
+        <v>333</v>
+      </c>
+      <c r="M137" t="s">
+        <v>218</v>
+      </c>
+      <c r="N137" t="s">
+        <v>448</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>546</v>
+      </c>
+      <c r="S137" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>91</v>
+      </c>
+      <c r="N138" t="s">
         <v>222</v>
       </c>
-      <c r="J40" t="s">
-        <v>222</v>
-      </c>
-      <c r="K40" t="s">
-        <v>337</v>
-      </c>
-      <c r="M40" t="s">
-        <v>415</v>
-      </c>
-      <c r="N40" t="s">
-        <v>454</v>
-      </c>
-      <c r="P40" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-      <c r="M41" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-      <c r="J42" t="s">
-        <v>284</v>
-      </c>
-      <c r="K42" t="s">
-        <v>222</v>
-      </c>
-      <c r="M42" t="s">
-        <v>447</v>
-      </c>
-      <c r="N42" t="s">
-        <v>457</v>
-      </c>
-      <c r="O42" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>92</v>
-      </c>
-      <c r="G44" t="s">
-        <v>92</v>
-      </c>
-      <c r="K44" t="s">
-        <v>334</v>
-      </c>
-      <c r="M44" t="s">
-        <v>437</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>438</v>
-      </c>
-      <c r="M45" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>440</v>
-      </c>
-      <c r="M46" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>442</v>
-      </c>
-      <c r="M47" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>44</v>
-      </c>
-      <c r="G48" t="s">
-        <v>257</v>
-      </c>
-      <c r="J48" t="s">
-        <v>268</v>
-      </c>
-      <c r="N48" t="s">
-        <v>339</v>
-      </c>
-      <c r="P48" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>45</v>
-      </c>
-      <c r="H49" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>531</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>533</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>186</v>
-      </c>
-      <c r="B52" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>46</v>
-      </c>
-      <c r="B53" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>47</v>
-      </c>
-      <c r="H54" t="s">
-        <v>223</v>
-      </c>
-      <c r="P54" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>48</v>
-      </c>
-      <c r="B55" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>49</v>
-      </c>
-      <c r="H56" t="s">
-        <v>188</v>
-      </c>
-      <c r="P56" t="s">
-        <v>516</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>469</v>
-      </c>
-      <c r="O57" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>51</v>
-      </c>
-      <c r="J59" t="s">
-        <v>318</v>
-      </c>
-      <c r="K59" t="s">
-        <v>176</v>
-      </c>
-      <c r="L59" t="s">
-        <v>396</v>
-      </c>
-      <c r="M59" t="s">
-        <v>436</v>
-      </c>
-      <c r="N59" t="s">
-        <v>453</v>
-      </c>
-      <c r="P59" t="s">
-        <v>510</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>459</v>
-      </c>
-      <c r="N60" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>315</v>
-      </c>
-      <c r="J61" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>52</v>
-      </c>
-      <c r="K62" t="s">
-        <v>325</v>
-      </c>
-      <c r="N62" t="s">
-        <v>451</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>53</v>
-      </c>
-      <c r="H63" t="s">
-        <v>212</v>
-      </c>
-      <c r="I63" t="s">
-        <v>212</v>
-      </c>
-      <c r="J63" t="s">
-        <v>212</v>
-      </c>
-      <c r="O63" t="s">
-        <v>503</v>
-      </c>
-      <c r="P63" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>271</v>
-      </c>
-      <c r="J64" t="s">
-        <v>272</v>
-      </c>
-      <c r="P64" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>54</v>
-      </c>
-      <c r="H65" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>55</v>
-      </c>
-      <c r="K66" t="s">
-        <v>212</v>
-      </c>
-      <c r="M66" t="s">
-        <v>212</v>
-      </c>
-      <c r="N66" t="s">
-        <v>212</v>
-      </c>
-      <c r="O66" t="s">
-        <v>502</v>
-      </c>
-      <c r="P66" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>401</v>
-      </c>
-      <c r="L67" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>56</v>
-      </c>
-      <c r="B68" t="s">
-        <v>175</v>
-      </c>
-      <c r="G68" t="s">
-        <v>195</v>
-      </c>
-      <c r="I68" t="s">
-        <v>175</v>
-      </c>
-      <c r="K68" t="s">
-        <v>175</v>
-      </c>
-      <c r="L68" t="s">
-        <v>175</v>
-      </c>
-      <c r="M68" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>57</v>
-      </c>
-      <c r="H69" t="s">
-        <v>224</v>
-      </c>
-      <c r="J69" t="s">
-        <v>266</v>
-      </c>
-      <c r="M69" t="s">
-        <v>445</v>
-      </c>
-      <c r="P69" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>58</v>
-      </c>
-      <c r="H70" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>59</v>
-      </c>
-      <c r="G71" t="s">
-        <v>196</v>
-      </c>
-      <c r="I71" t="s">
-        <v>243</v>
-      </c>
-      <c r="L71" t="s">
-        <v>395</v>
-      </c>
-      <c r="N71" t="s">
-        <v>452</v>
-      </c>
-      <c r="O71" t="s">
-        <v>471</v>
-      </c>
-      <c r="P71" t="s">
-        <v>514</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>202</v>
-      </c>
-      <c r="G72" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>61</v>
-      </c>
-      <c r="H74" t="s">
-        <v>208</v>
-      </c>
-      <c r="O74" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>245</v>
-      </c>
-      <c r="I75" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>319</v>
-      </c>
-      <c r="J76" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>63</v>
-      </c>
-      <c r="K78" t="s">
-        <v>331</v>
-      </c>
-      <c r="M78" t="s">
-        <v>298</v>
-      </c>
-      <c r="N78" t="s">
-        <v>298</v>
-      </c>
-      <c r="O78" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>64</v>
-      </c>
-      <c r="J79" t="s">
-        <v>298</v>
-      </c>
-      <c r="K79" t="s">
-        <v>323</v>
-      </c>
-      <c r="M79" t="s">
-        <v>298</v>
-      </c>
-      <c r="N79" t="s">
-        <v>298</v>
-      </c>
-      <c r="O79" t="s">
-        <v>323</v>
-      </c>
-      <c r="Q79" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>427</v>
-      </c>
-      <c r="M80" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>65</v>
-      </c>
-      <c r="H81" t="s">
-        <v>217</v>
-      </c>
-      <c r="K81" t="s">
-        <v>339</v>
-      </c>
-      <c r="M81" t="s">
-        <v>433</v>
-      </c>
-      <c r="P81" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>307</v>
-      </c>
-      <c r="J82" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>66</v>
-      </c>
-      <c r="J83" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>299</v>
-      </c>
-      <c r="J84" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>67</v>
-      </c>
-      <c r="G85" t="s">
-        <v>265</v>
-      </c>
-      <c r="M85" t="s">
-        <v>419</v>
-      </c>
-      <c r="N85" t="s">
-        <v>419</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>311</v>
-      </c>
-      <c r="J86" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>309</v>
-      </c>
-      <c r="J87" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>305</v>
-      </c>
-      <c r="J88" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>68</v>
-      </c>
-      <c r="B89" t="s">
-        <v>183</v>
-      </c>
-      <c r="I89" t="s">
-        <v>247</v>
-      </c>
-      <c r="N89" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>69</v>
-      </c>
-      <c r="H90" t="s">
-        <v>233</v>
-      </c>
-      <c r="J90" t="s">
-        <v>278</v>
-      </c>
-      <c r="K90" t="s">
-        <v>328</v>
-      </c>
-      <c r="M90" t="s">
-        <v>444</v>
-      </c>
-      <c r="N90" t="s">
-        <v>449</v>
-      </c>
-      <c r="P90" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q90" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>70</v>
-      </c>
-      <c r="L91" t="s">
-        <v>263</v>
-      </c>
-      <c r="M91" t="s">
-        <v>411</v>
-      </c>
-      <c r="N91" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>71</v>
-      </c>
-      <c r="J92" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>72</v>
-      </c>
-      <c r="J93" t="s">
-        <v>314</v>
-      </c>
-      <c r="N93" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>73</v>
-      </c>
-      <c r="H94" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>74</v>
-      </c>
-      <c r="B95" t="s">
-        <v>173</v>
-      </c>
-      <c r="I95" t="s">
-        <v>252</v>
-      </c>
-      <c r="J95" t="s">
-        <v>277</v>
-      </c>
-      <c r="K95" t="s">
-        <v>336</v>
-      </c>
-      <c r="M95" t="s">
-        <v>446</v>
-      </c>
-      <c r="Q95" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>269</v>
-      </c>
-      <c r="J96" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>496</v>
-      </c>
-      <c r="O97" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>498</v>
-      </c>
-      <c r="O98" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>303</v>
-      </c>
-      <c r="J99" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>219</v>
-      </c>
-      <c r="H100" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>75</v>
-      </c>
-      <c r="J101" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>76</v>
-      </c>
-      <c r="H102" t="s">
-        <v>232</v>
-      </c>
-      <c r="K102" t="s">
-        <v>342</v>
-      </c>
-      <c r="L102" t="s">
-        <v>342</v>
-      </c>
-      <c r="N102" t="s">
-        <v>342</v>
-      </c>
-      <c r="O102" t="s">
-        <v>494</v>
-      </c>
-      <c r="Q102" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>77</v>
-      </c>
-      <c r="G103" t="s">
-        <v>197</v>
-      </c>
-      <c r="H103" t="s">
-        <v>224</v>
-      </c>
-      <c r="I103" t="s">
-        <v>239</v>
-      </c>
-      <c r="J103" t="s">
-        <v>239</v>
-      </c>
-      <c r="K103" t="s">
-        <v>324</v>
-      </c>
-      <c r="L103" t="s">
-        <v>407</v>
-      </c>
-      <c r="N103" t="s">
-        <v>458</v>
-      </c>
-      <c r="O103" t="s">
-        <v>495</v>
-      </c>
-      <c r="P103" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>78</v>
-      </c>
-      <c r="H104" t="s">
-        <v>216</v>
-      </c>
-      <c r="J104" t="s">
-        <v>286</v>
-      </c>
-      <c r="K104" t="s">
-        <v>338</v>
-      </c>
-      <c r="L104" t="s">
-        <v>216</v>
-      </c>
-      <c r="M104" t="s">
-        <v>432</v>
-      </c>
-      <c r="P104" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>80</v>
-      </c>
-      <c r="J106" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q106" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>81</v>
-      </c>
-      <c r="K107" t="s">
-        <v>329</v>
-      </c>
-      <c r="M107" t="s">
-        <v>412</v>
-      </c>
-      <c r="N107" t="s">
-        <v>412</v>
-      </c>
-      <c r="Q107" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>261</v>
-      </c>
-      <c r="G108" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>82</v>
-      </c>
-      <c r="B109" t="s">
-        <v>182</v>
-      </c>
-      <c r="H109" t="s">
-        <v>225</v>
-      </c>
-      <c r="I109" t="s">
-        <v>182</v>
-      </c>
-      <c r="J109" t="s">
-        <v>225</v>
-      </c>
-      <c r="K109" t="s">
-        <v>322</v>
-      </c>
-      <c r="M109" t="s">
-        <v>182</v>
-      </c>
-      <c r="N109" t="s">
-        <v>182</v>
-      </c>
-      <c r="P109" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>83</v>
-      </c>
-      <c r="H110" t="s">
-        <v>216</v>
-      </c>
-      <c r="I110" t="s">
-        <v>242</v>
-      </c>
-      <c r="J110" t="s">
-        <v>216</v>
-      </c>
-      <c r="P110" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q110" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>84</v>
-      </c>
-      <c r="J111" t="s">
-        <v>267</v>
-      </c>
-      <c r="M111" t="s">
-        <v>420</v>
-      </c>
-      <c r="Q111" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>279</v>
-      </c>
-      <c r="J116" t="s">
-        <v>280</v>
-      </c>
-      <c r="O116" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>177</v>
-      </c>
-      <c r="B117" t="s">
-        <v>179</v>
-      </c>
-      <c r="O117" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>193</v>
-      </c>
-      <c r="G118" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q119" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>466</v>
-      </c>
-      <c r="N120" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>178</v>
-      </c>
-      <c r="B121" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>464</v>
-      </c>
-      <c r="N122" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>90</v>
-      </c>
-      <c r="H123" t="s">
-        <v>218</v>
-      </c>
-      <c r="K123" t="s">
-        <v>333</v>
-      </c>
-      <c r="M123" t="s">
-        <v>218</v>
-      </c>
-      <c r="N123" t="s">
-        <v>448</v>
-      </c>
-      <c r="Q123" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>91</v>
-      </c>
-      <c r="N124" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q124" t="s">
+      <c r="Q138" t="s">
         <v>519</v>
       </c>
     </row>

</xml_diff>